<commit_message>
added fraction of fishery per fleet for lingcod 2017
</commit_message>
<xml_diff>
--- a/data/Selectivity parameters/fraction_of_fishery.xlsx
+++ b/data/Selectivity parameters/fraction_of_fishery.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vique\Documents\Projects\DensityRatio\data\Selectivity parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vic\Documents\Projects\DensityRatio\data\Selectivity parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EB1576-4010-4D9E-BC3B-D425A42ED96D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596486B5-6927-4A06-8EA6-ED9D85229404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="20400" windowHeight="7875" xr2:uid="{61ABCC0D-E7EA-4BC2-A5B0-7613055FF009}"/>
+    <workbookView xWindow="-24825" yWindow="7260" windowWidth="13830" windowHeight="7170" xr2:uid="{61ABCC0D-E7EA-4BC2-A5B0-7613055FF009}"/>
   </bookViews>
   <sheets>
-    <sheet name="CAB2005" sheetId="6" r:id="rId1"/>
-    <sheet name="BR 2015" sheetId="4" r:id="rId2"/>
-    <sheet name="BR 2003" sheetId="5" r:id="rId3"/>
-    <sheet name="CAB2019" sheetId="3" r:id="rId4"/>
-    <sheet name="lingcod" sheetId="2" r:id="rId5"/>
-    <sheet name="copper rockfish" sheetId="1" r:id="rId6"/>
+    <sheet name="LING2017" sheetId="7" r:id="rId1"/>
+    <sheet name="CAB2005" sheetId="6" r:id="rId2"/>
+    <sheet name="BR 2015" sheetId="4" r:id="rId3"/>
+    <sheet name="BR 2003" sheetId="5" r:id="rId4"/>
+    <sheet name="CAB2019" sheetId="3" r:id="rId5"/>
+    <sheet name="lingcod" sheetId="2" r:id="rId6"/>
+    <sheet name="copper rockfish" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Years</t>
   </si>
@@ -136,6 +139,21 @@
   <si>
     <t>averages</t>
   </si>
+  <si>
+    <t>Trawl</t>
+  </si>
+  <si>
+    <t>Fixed Gear</t>
+  </si>
+  <si>
+    <t>WA rec</t>
+  </si>
+  <si>
+    <t>OR rec</t>
+  </si>
+  <si>
+    <t>Total catch</t>
+  </si>
 </sst>
 </file>
 
@@ -193,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -208,6 +226,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,24 +543,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F2C116-E186-401B-9D63-CD4A71AC94B0}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>2005</v>
+      </c>
+      <c r="B2" s="6">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="C2" s="6">
+        <v>58.01</v>
+      </c>
+      <c r="D2" s="6">
+        <v>78.31</v>
+      </c>
+      <c r="E2" s="6">
+        <v>140.84</v>
+      </c>
+      <c r="F2" s="6">
+        <v>356.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2006</v>
+      </c>
+      <c r="B3" s="6">
+        <v>115.58</v>
+      </c>
+      <c r="C3" s="6">
+        <v>78.63</v>
+      </c>
+      <c r="D3" s="6">
+        <v>62.18</v>
+      </c>
+      <c r="E3" s="6">
+        <v>107.61</v>
+      </c>
+      <c r="F3" s="6">
+        <v>364.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2007</v>
+      </c>
+      <c r="B4" s="6">
+        <v>113.63</v>
+      </c>
+      <c r="C4" s="6">
+        <v>71.17</v>
+      </c>
+      <c r="D4" s="6">
+        <v>68.209999999999994</v>
+      </c>
+      <c r="E4" s="6">
+        <v>104.02</v>
+      </c>
+      <c r="F4" s="6">
+        <v>357.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="6">
+        <v>118.79</v>
+      </c>
+      <c r="C5" s="6">
+        <v>92.78</v>
+      </c>
+      <c r="D5" s="6">
+        <v>70.81</v>
+      </c>
+      <c r="E5" s="6">
+        <v>89.34</v>
+      </c>
+      <c r="F5" s="6">
+        <v>371.72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>2009</v>
+      </c>
+      <c r="B6" s="6">
+        <v>93.47</v>
+      </c>
+      <c r="C6" s="6">
+        <v>81.47</v>
+      </c>
+      <c r="D6" s="6">
+        <v>74.25</v>
+      </c>
+      <c r="E6" s="6">
+        <v>78.760000000000005</v>
+      </c>
+      <c r="F6" s="6">
+        <v>327.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>2010</v>
+      </c>
+      <c r="B7" s="6">
+        <v>77.760000000000005</v>
+      </c>
+      <c r="C7" s="6">
+        <v>47.22</v>
+      </c>
+      <c r="D7" s="6">
+        <v>91.43</v>
+      </c>
+      <c r="E7" s="6">
+        <v>93.94</v>
+      </c>
+      <c r="F7" s="6">
+        <v>310.35000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>2011</v>
+      </c>
+      <c r="B8" s="6">
+        <v>283.43</v>
+      </c>
+      <c r="C8" s="6">
+        <v>57.64</v>
+      </c>
+      <c r="D8" s="6">
+        <v>117.78</v>
+      </c>
+      <c r="E8" s="6">
+        <v>114.99</v>
+      </c>
+      <c r="F8" s="6">
+        <v>573.83000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>2012</v>
+      </c>
+      <c r="B9" s="6">
+        <v>373.23</v>
+      </c>
+      <c r="C9" s="6">
+        <v>64.87</v>
+      </c>
+      <c r="D9" s="6">
+        <v>122.32</v>
+      </c>
+      <c r="E9" s="6">
+        <v>155.25</v>
+      </c>
+      <c r="F9" s="6">
+        <v>715.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="6">
+        <v>360.35</v>
+      </c>
+      <c r="C10" s="6">
+        <v>78.34</v>
+      </c>
+      <c r="D10" s="6">
+        <v>127.32</v>
+      </c>
+      <c r="E10" s="6">
+        <v>224</v>
+      </c>
+      <c r="F10" s="6">
+        <v>790.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>2014</v>
+      </c>
+      <c r="B11" s="6">
+        <v>217.53</v>
+      </c>
+      <c r="C11" s="6">
+        <v>82.2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>141.58000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>176.09</v>
+      </c>
+      <c r="F11" s="6">
+        <v>617.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="6">
+        <v>163.4</v>
+      </c>
+      <c r="C12" s="6">
+        <v>132.54</v>
+      </c>
+      <c r="D12" s="6">
+        <v>271.95</v>
+      </c>
+      <c r="E12" s="6">
+        <v>226.17</v>
+      </c>
+      <c r="F12" s="6">
+        <v>794.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>2016</v>
+      </c>
+      <c r="B13" s="6">
+        <v>262.74</v>
+      </c>
+      <c r="C13" s="6">
+        <v>98.31</v>
+      </c>
+      <c r="D13" s="6">
+        <v>349.69</v>
+      </c>
+      <c r="E13" s="6">
+        <v>154.66</v>
+      </c>
+      <c r="F13" s="6">
+        <v>865.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f>B2/$F2</f>
+        <v>0.2225089766606822</v>
+      </c>
+      <c r="C18">
+        <f>C2/$F2</f>
+        <v>0.16273002692998204</v>
+      </c>
+      <c r="D18">
+        <f>D2/$F2</f>
+        <v>0.21967571813285458</v>
+      </c>
+      <c r="E18">
+        <f>E2/$F2</f>
+        <v>0.39508527827648116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f>B3/$F3</f>
+        <v>0.31751874948490427</v>
+      </c>
+      <c r="C19">
+        <f>C3/$F3</f>
+        <v>0.21601054916073734</v>
+      </c>
+      <c r="D19">
+        <f>D3/$F3</f>
+        <v>0.17081948298123678</v>
+      </c>
+      <c r="E19">
+        <f>E3/$F3</f>
+        <v>0.29562374660036811</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>B4/$F4</f>
+        <v>0.31826457160462707</v>
+      </c>
+      <c r="C20">
+        <f>C4/$F4</f>
+        <v>0.19933899112119433</v>
+      </c>
+      <c r="D20">
+        <f>D4/$F4</f>
+        <v>0.19104837128532617</v>
+      </c>
+      <c r="E20">
+        <f>E4/$F4</f>
+        <v>0.29134806598885249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>B5/$F5</f>
+        <v>0.31956849241364466</v>
+      </c>
+      <c r="C21">
+        <f>C5/$F5</f>
+        <v>0.24959647046163777</v>
+      </c>
+      <c r="D21">
+        <f>D5/$F5</f>
+        <v>0.19049284407618636</v>
+      </c>
+      <c r="E21">
+        <f>E5/$F5</f>
+        <v>0.24034219304853113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>B6/$F6</f>
+        <v>0.28501295929257509</v>
+      </c>
+      <c r="C22">
+        <f>C6/$F6</f>
+        <v>0.24842201555115109</v>
+      </c>
+      <c r="D22">
+        <f>D6/$F6</f>
+        <v>0.22640646440006099</v>
+      </c>
+      <c r="E22">
+        <f>E6/$F6</f>
+        <v>0.24015856075621286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>B7/$F7</f>
+        <v>0.25055582406959886</v>
+      </c>
+      <c r="C23">
+        <f>C7/$F7</f>
+        <v>0.15215079748670854</v>
+      </c>
+      <c r="D23">
+        <f>D7/$F7</f>
+        <v>0.29460286772998229</v>
+      </c>
+      <c r="E23">
+        <f>E7/$F7</f>
+        <v>0.30269051071371028</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f>B8/$F8</f>
+        <v>0.49392677273757035</v>
+      </c>
+      <c r="C24">
+        <f>C8/$F8</f>
+        <v>0.10044786783542163</v>
+      </c>
+      <c r="D24">
+        <f>D8/$F8</f>
+        <v>0.20525242667689036</v>
+      </c>
+      <c r="E24">
+        <f>E8/$F8</f>
+        <v>0.2003903595141418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <f>B9/$F9</f>
+        <v>0.52150402414486929</v>
+      </c>
+      <c r="C25">
+        <f>C9/$F9</f>
+        <v>9.0641068634026392E-2</v>
+      </c>
+      <c r="D25">
+        <f>D9/$F9</f>
+        <v>0.17091437513972726</v>
+      </c>
+      <c r="E25">
+        <f>E9/$F9</f>
+        <v>0.21692655935613683</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f>B10/$F10</f>
+        <v>0.45613346666497895</v>
+      </c>
+      <c r="C26">
+        <f>C10/$F10</f>
+        <v>9.9163301730357853E-2</v>
+      </c>
+      <c r="D26">
+        <f>D10/$F10</f>
+        <v>0.16116251693016542</v>
+      </c>
+      <c r="E26">
+        <f>E10/$F10</f>
+        <v>0.28354071467449782</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f>B11/$F11</f>
+        <v>0.35232665489707005</v>
+      </c>
+      <c r="C27">
+        <f>C11/$F11</f>
+        <v>0.13313681346269093</v>
+      </c>
+      <c r="D27">
+        <f>D11/$F11</f>
+        <v>0.22931277433148153</v>
+      </c>
+      <c r="E27">
+        <f>E11/$F11</f>
+        <v>0.28520756061612224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <f>B12/$F12</f>
+        <v>0.20577530948153186</v>
+      </c>
+      <c r="C28">
+        <f>C12/$F12</f>
+        <v>0.16691223695643959</v>
+      </c>
+      <c r="D28">
+        <f>D12/$F12</f>
+        <v>0.34247610412180285</v>
+      </c>
+      <c r="E28">
+        <f>E12/$F12</f>
+        <v>0.28482375609203214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <f>B13/$F13</f>
+        <v>0.30360526923965797</v>
+      </c>
+      <c r="C29">
+        <f>C13/$F13</f>
+        <v>0.11360064709960713</v>
+      </c>
+      <c r="D29">
+        <f>D13/$F13</f>
+        <v>0.40407903859486943</v>
+      </c>
+      <c r="E29">
+        <f>E13/$F13</f>
+        <v>0.1787150450658655</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(B27:B29)</f>
+        <v>0.28723574453941997</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:E31" si="0">AVERAGE(C27:C29)</f>
+        <v>0.1378832325062459</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.32528930568271797</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.24958212059133991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7241E4D-5FAA-4EB0-9CA5-442B065A2EF9}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +1128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2002</v>
       </c>
@@ -592,7 +1155,7 @@
         <v>17891</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2003</v>
       </c>
@@ -619,7 +1182,7 @@
         <v>15814</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2004</v>
       </c>
@@ -646,7 +1209,7 @@
         <v>12796</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -654,90 +1217,90 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <f>B2/$H2</f>
+        <f t="shared" ref="B6:G6" si="1">B2/$H2</f>
         <v>1.9954166899558437E-2</v>
       </c>
       <c r="C6" s="1">
-        <f>C2/$H2</f>
+        <f t="shared" si="1"/>
         <v>0.35548599854675533</v>
       </c>
       <c r="D6" s="1">
-        <f>D2/$H2</f>
+        <f t="shared" si="1"/>
         <v>0.10189480744508413</v>
       </c>
       <c r="E6" s="1">
-        <f>E2/$H2</f>
+        <f t="shared" si="1"/>
         <v>9.6696663126711758E-3</v>
       </c>
       <c r="F6" s="1">
-        <f>F2/$H2</f>
+        <f t="shared" si="1"/>
         <v>0.19311385612877982</v>
       </c>
       <c r="G6" s="1">
-        <f>G2/$H2</f>
+        <f t="shared" si="1"/>
         <v>0.3198815046671511</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
-        <f t="shared" ref="B7:G7" si="1">B3/$H3</f>
+        <f t="shared" ref="B7:G7" si="2">B3/$H3</f>
         <v>2.2827874035664601E-2</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34191222966991275</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3280637409889974E-2</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1996964714809666E-2</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11755406601745289</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.40242822815227014</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:G8" si="2">B4/$H4</f>
+        <f t="shared" ref="B8:G8" si="3">B4/$H4</f>
         <v>1.3050953422944669E-2</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.31916223819943734</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17708658955923726</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0556423882463268E-2</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28071272272585185</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17943107221006566</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -745,7 +1308,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -754,23 +1317,23 @@
         <v>1.8610998119389235E-2</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ref="C10:G10" si="3">AVERAGE(C6:C8)</f>
+        <f t="shared" ref="C10:G10" si="4">AVERAGE(C6:C8)</f>
         <v>0.33885348880536847</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12075401147140379</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4074351636648034E-2</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19712688162402822</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.30058026834316226</v>
       </c>
       <c r="I10" s="1">
@@ -778,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -786,7 +1349,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -794,7 +1357,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -802,7 +1365,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="19" spans="2:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -813,7 +1376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C517727F-A68E-482A-9E07-1F760117E79A}">
   <dimension ref="A1:M130"/>
   <sheetViews>
@@ -821,12 +1384,12 @@
       <selection activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -849,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1892</v>
       </c>
@@ -873,7 +1436,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1893</v>
       </c>
@@ -897,7 +1460,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1894</v>
       </c>
@@ -921,7 +1484,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1895</v>
       </c>
@@ -945,7 +1508,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1896</v>
       </c>
@@ -969,7 +1532,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1897</v>
       </c>
@@ -993,7 +1556,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>1898</v>
       </c>
@@ -1017,7 +1580,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1899</v>
       </c>
@@ -1041,7 +1604,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1900</v>
       </c>
@@ -1065,7 +1628,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>1901</v>
       </c>
@@ -1089,7 +1652,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1902</v>
       </c>
@@ -1113,7 +1676,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>1903</v>
       </c>
@@ -1137,7 +1700,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>1904</v>
       </c>
@@ -1161,7 +1724,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>1905</v>
       </c>
@@ -1185,7 +1748,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>1906</v>
       </c>
@@ -1209,7 +1772,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>1907</v>
       </c>
@@ -1233,7 +1796,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>1908</v>
       </c>
@@ -1257,7 +1820,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>1909</v>
       </c>
@@ -1281,7 +1844,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>1910</v>
       </c>
@@ -1305,7 +1868,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>1911</v>
       </c>
@@ -1329,7 +1892,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>1912</v>
       </c>
@@ -1353,7 +1916,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>1913</v>
       </c>
@@ -1377,7 +1940,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>1914</v>
       </c>
@@ -1401,7 +1964,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>1915</v>
       </c>
@@ -1425,7 +1988,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>1916</v>
       </c>
@@ -1449,7 +2012,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>1917</v>
       </c>
@@ -1473,7 +2036,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>1918</v>
       </c>
@@ -1497,7 +2060,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>1919</v>
       </c>
@@ -1521,7 +2084,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>1920</v>
       </c>
@@ -1545,7 +2108,7 @@
         <v>2.9499999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>1921</v>
       </c>
@@ -1569,7 +2132,7 @@
         <v>1.8499999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>1922</v>
       </c>
@@ -1593,7 +2156,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>1923</v>
       </c>
@@ -1617,7 +2180,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>1924</v>
       </c>
@@ -1641,7 +2204,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>1925</v>
       </c>
@@ -1665,7 +2228,7 @@
         <v>2.3200000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>1926</v>
       </c>
@@ -1689,7 +2252,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>1927</v>
       </c>
@@ -1713,7 +2276,7 @@
         <v>2.4499999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>1928</v>
       </c>
@@ -1737,7 +2300,7 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>1929</v>
       </c>
@@ -1761,7 +2324,7 @@
         <v>3.23</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>1930</v>
       </c>
@@ -1785,7 +2348,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>1931</v>
       </c>
@@ -1809,7 +2372,7 @@
         <v>2.9299999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>1932</v>
       </c>
@@ -1833,7 +2396,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>1933</v>
       </c>
@@ -1857,7 +2420,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>1934</v>
       </c>
@@ -1881,7 +2444,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>1935</v>
       </c>
@@ -1905,7 +2468,7 @@
         <v>2.4899999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>1936</v>
       </c>
@@ -1929,7 +2492,7 @@
         <v>3.7199999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>1937</v>
       </c>
@@ -1953,7 +2516,7 @@
         <v>5.3100000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>1938</v>
       </c>
@@ -1977,7 +2540,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>1939</v>
       </c>
@@ -2001,7 +2564,7 @@
         <v>6.13</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>1940</v>
       </c>
@@ -2025,7 +2588,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>1941</v>
       </c>
@@ -2049,7 +2612,7 @@
         <v>8.4499999999999993</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>1942</v>
       </c>
@@ -2073,7 +2636,7 @@
         <v>10.92</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>1943</v>
       </c>
@@ -2097,7 +2660,7 @@
         <v>37.53</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>1944</v>
       </c>
@@ -2121,7 +2684,7 @@
         <v>77.92</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>1945</v>
       </c>
@@ -2145,7 +2708,7 @@
         <v>125.65</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>1946</v>
       </c>
@@ -2169,7 +2732,7 @@
         <v>92.22</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>1947</v>
       </c>
@@ -2193,7 +2756,7 @@
         <v>33.92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>1948</v>
       </c>
@@ -2217,7 +2780,7 @@
         <v>24.970000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>1949</v>
       </c>
@@ -2241,7 +2804,7 @@
         <v>12.989999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>1950</v>
       </c>
@@ -2265,7 +2828,7 @@
         <v>61.67</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>1951</v>
       </c>
@@ -2289,7 +2852,7 @@
         <v>22.17</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>1952</v>
       </c>
@@ -2313,7 +2876,7 @@
         <v>13.969999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>1953</v>
       </c>
@@ -2337,7 +2900,7 @@
         <v>26.740000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>1954</v>
       </c>
@@ -2361,7 +2924,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>1955</v>
       </c>
@@ -2385,7 +2948,7 @@
         <v>41.14</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>1956</v>
       </c>
@@ -2410,7 +2973,7 @@
       </c>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>1957</v>
       </c>
@@ -2435,7 +2998,7 @@
       </c>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>1958</v>
       </c>
@@ -2460,7 +3023,7 @@
       </c>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>1959</v>
       </c>
@@ -2485,7 +3048,7 @@
       </c>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>1960</v>
       </c>
@@ -2510,7 +3073,7 @@
       </c>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>1961</v>
       </c>
@@ -2535,7 +3098,7 @@
       </c>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>1962</v>
       </c>
@@ -2560,7 +3123,7 @@
       </c>
       <c r="M72" s="4"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>1963</v>
       </c>
@@ -2585,7 +3148,7 @@
       </c>
       <c r="M73" s="4"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>1964</v>
       </c>
@@ -2610,7 +3173,7 @@
       </c>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>1965</v>
       </c>
@@ -2635,7 +3198,7 @@
       </c>
       <c r="M75" s="4"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>1966</v>
       </c>
@@ -2660,7 +3223,7 @@
       </c>
       <c r="M76" s="4"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>1967</v>
       </c>
@@ -2685,7 +3248,7 @@
       </c>
       <c r="M77" s="4"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>1968</v>
       </c>
@@ -2710,7 +3273,7 @@
       </c>
       <c r="M78" s="4"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>1969</v>
       </c>
@@ -2735,7 +3298,7 @@
       </c>
       <c r="M79" s="4"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>1970</v>
       </c>
@@ -2760,7 +3323,7 @@
       </c>
       <c r="M80" s="4"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>1971</v>
       </c>
@@ -2785,7 +3348,7 @@
       </c>
       <c r="M81" s="4"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>1972</v>
       </c>
@@ -2810,7 +3373,7 @@
       </c>
       <c r="M82" s="4"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>1973</v>
       </c>
@@ -2835,7 +3398,7 @@
       </c>
       <c r="M83" s="4"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>1974</v>
       </c>
@@ -2860,7 +3423,7 @@
       </c>
       <c r="M84" s="4"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>1975</v>
       </c>
@@ -2885,7 +3448,7 @@
       </c>
       <c r="M85" s="4"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>1976</v>
       </c>
@@ -2910,7 +3473,7 @@
       </c>
       <c r="M86" s="4"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>1977</v>
       </c>
@@ -2935,7 +3498,7 @@
       </c>
       <c r="M87" s="4"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>1978</v>
       </c>
@@ -2960,7 +3523,7 @@
       </c>
       <c r="M88" s="4"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>1979</v>
       </c>
@@ -2985,7 +3548,7 @@
       </c>
       <c r="M89" s="4"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>1980</v>
       </c>
@@ -3010,7 +3573,7 @@
       </c>
       <c r="M90" s="4"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>1981</v>
       </c>
@@ -3035,7 +3598,7 @@
       </c>
       <c r="M91" s="4"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>1982</v>
       </c>
@@ -3060,7 +3623,7 @@
       </c>
       <c r="M92" s="4"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>1983</v>
       </c>
@@ -3085,7 +3648,7 @@
       </c>
       <c r="M93" s="4"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>1984</v>
       </c>
@@ -3110,7 +3673,7 @@
       </c>
       <c r="M94" s="4"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>1985</v>
       </c>
@@ -3138,7 +3701,7 @@
       <c r="L95" s="6"/>
       <c r="M95" s="6"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>1986</v>
       </c>
@@ -3162,7 +3725,7 @@
         <v>252.17999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>1987</v>
       </c>
@@ -3186,7 +3749,7 @@
         <v>251.77000000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>1988</v>
       </c>
@@ -3210,7 +3773,7 @@
         <v>318.28000000000003</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>1989</v>
       </c>
@@ -3234,7 +3797,7 @@
         <v>394.46000000000004</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>1990</v>
       </c>
@@ -3258,7 +3821,7 @@
         <v>365.55999999999995</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>1991</v>
       </c>
@@ -3282,7 +3845,7 @@
         <v>270.77999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>1992</v>
       </c>
@@ -3306,7 +3869,7 @@
         <v>644.7600000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>1993</v>
       </c>
@@ -3330,7 +3893,7 @@
         <v>451.24</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>1994</v>
       </c>
@@ -3354,7 +3917,7 @@
         <v>451.21999999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>1995</v>
       </c>
@@ -3378,7 +3941,7 @@
         <v>455.54000000000008</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>1996</v>
       </c>
@@ -3402,7 +3965,7 @@
         <v>527.44000000000005</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>1997</v>
       </c>
@@ -3426,7 +3989,7 @@
         <v>509.22</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>1998</v>
       </c>
@@ -3450,7 +4013,7 @@
         <v>470.55</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <v>1999</v>
       </c>
@@ -3474,7 +4037,7 @@
         <v>408.14</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
         <v>2000</v>
       </c>
@@ -3498,7 +4061,7 @@
         <v>418.32000000000005</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
         <v>2001</v>
       </c>
@@ -3522,7 +4085,7 @@
         <v>471.49</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <v>2002</v>
       </c>
@@ -3546,7 +4109,7 @@
         <v>429.64</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <v>2003</v>
       </c>
@@ -3570,7 +4133,7 @@
         <v>474.42999999999995</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <v>2004</v>
       </c>
@@ -3594,7 +4157,7 @@
         <v>463.66</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <v>2005</v>
       </c>
@@ -3618,7 +4181,7 @@
         <v>427.37</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>2006</v>
       </c>
@@ -3642,7 +4205,7 @@
         <v>375.71</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>2007</v>
       </c>
@@ -3666,7 +4229,7 @@
         <v>374.19000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <v>2008</v>
       </c>
@@ -3690,7 +4253,7 @@
         <v>353.22999999999996</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <v>2009</v>
       </c>
@@ -3714,7 +4277,7 @@
         <v>445.71</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <v>2010</v>
       </c>
@@ -3738,7 +4301,7 @@
         <v>419.6</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <v>2011</v>
       </c>
@@ -3762,7 +4325,7 @@
         <v>319.45999999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>2012</v>
       </c>
@@ -3786,7 +4349,7 @@
         <v>330.26</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>2013</v>
       </c>
@@ -3810,7 +4373,7 @@
         <v>436.28999999999996</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <v>2014</v>
       </c>
@@ -3834,7 +4397,7 @@
         <v>485.34</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>24</v>
       </c>
@@ -3859,7 +4422,7 @@
         <v>4.4601223278628963E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="3">
         <f t="shared" ref="B127:F127" si="3">B123/$G123</f>
@@ -3882,7 +4445,7 @@
         <v>3.3303536638474414E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="3">
         <f t="shared" ref="B128:F128" si="4">B124/$G124</f>
@@ -3905,10 +4468,10 @@
         <v>2.9525693328388346E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>25</v>
       </c>
@@ -3938,7 +4501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5261AC-2996-4C0A-8AE8-F2AF54AD1241}">
   <dimension ref="A1:H65"/>
   <sheetViews>
@@ -3946,9 +4509,9 @@
       <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3974,7 +4537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1945</v>
       </c>
@@ -4000,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1946</v>
       </c>
@@ -4026,7 +4589,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1947</v>
       </c>
@@ -4052,7 +4615,7 @@
         <v>78.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1948</v>
       </c>
@@ -4078,7 +4641,7 @@
         <v>118.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1949</v>
       </c>
@@ -4104,7 +4667,7 @@
         <v>157.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1950</v>
       </c>
@@ -4130,7 +4693,7 @@
         <v>196.8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1951</v>
       </c>
@@ -4156,7 +4719,7 @@
         <v>236.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1952</v>
       </c>
@@ -4182,7 +4745,7 @@
         <v>275.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1953</v>
       </c>
@@ -4208,7 +4771,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1954</v>
       </c>
@@ -4234,7 +4797,7 @@
         <v>354.2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1955</v>
       </c>
@@ -4260,7 +4823,7 @@
         <v>377.7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1956</v>
       </c>
@@ -4286,7 +4849,7 @@
         <v>426.9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1957</v>
       </c>
@@ -4312,7 +4875,7 @@
         <v>461.8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1958</v>
       </c>
@@ -4338,7 +4901,7 @@
         <v>480.7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1959</v>
       </c>
@@ -4364,7 +4927,7 @@
         <v>458.9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1960</v>
       </c>
@@ -4390,7 +4953,7 @@
         <v>467.2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1961</v>
       </c>
@@ -4416,7 +4979,7 @@
         <v>430.4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1962</v>
       </c>
@@ -4442,7 +5005,7 @@
         <v>425.7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1963</v>
       </c>
@@ -4468,7 +5031,7 @@
         <v>475.9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1964</v>
       </c>
@@ -4494,7 +5057,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1965</v>
       </c>
@@ -4520,7 +5083,7 @@
         <v>519.20000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1966</v>
       </c>
@@ -4546,7 +5109,7 @@
         <v>588.29999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1967</v>
       </c>
@@ -4572,7 +5135,7 @@
         <v>636.6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1968</v>
       </c>
@@ -4598,7 +5161,7 @@
         <v>573.6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1969</v>
       </c>
@@ -4624,7 +5187,7 @@
         <v>685.2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1970</v>
       </c>
@@ -4650,7 +5213,7 @@
         <v>775.3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1971</v>
       </c>
@@ -4676,7 +5239,7 @@
         <v>694.1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1972</v>
       </c>
@@ -4702,7 +5265,7 @@
         <v>742.5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1973</v>
       </c>
@@ -4728,7 +5291,7 @@
         <v>763.3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1974</v>
       </c>
@@ -4754,7 +5317,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1975</v>
       </c>
@@ -4780,7 +5343,7 @@
         <v>936.4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1976</v>
       </c>
@@ -4806,7 +5369,7 @@
         <v>1118.5999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1977</v>
       </c>
@@ -4832,7 +5395,7 @@
         <v>936.8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1978</v>
       </c>
@@ -4858,7 +5421,7 @@
         <v>1042.2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1979</v>
       </c>
@@ -4884,7 +5447,7 @@
         <v>1099.3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1980</v>
       </c>
@@ -4910,7 +5473,7 @@
         <v>734.1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1981</v>
       </c>
@@ -4936,7 +5499,7 @@
         <v>1835.8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1982</v>
       </c>
@@ -4962,7 +5525,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1983</v>
       </c>
@@ -4988,7 +5551,7 @@
         <v>1325.5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1984</v>
       </c>
@@ -5014,7 +5577,7 @@
         <v>1272.7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1985</v>
       </c>
@@ -5040,7 +5603,7 @@
         <v>1186.5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1986</v>
       </c>
@@ -5066,7 +5629,7 @@
         <v>815.8</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1987</v>
       </c>
@@ -5092,7 +5655,7 @@
         <v>663.8</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -5118,7 +5681,7 @@
         <v>915.9</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1989</v>
       </c>
@@ -5144,7 +5707,7 @@
         <v>1017.5</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -5170,7 +5733,7 @@
         <v>895.5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1991</v>
       </c>
@@ -5196,7 +5759,7 @@
         <v>711.3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1992</v>
       </c>
@@ -5222,7 +5785,7 @@
         <v>1194.2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -5248,7 +5811,7 @@
         <v>885.5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1994</v>
       </c>
@@ -5274,7 +5837,7 @@
         <v>846.6</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1995</v>
       </c>
@@ -5300,7 +5863,7 @@
         <v>857.8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1996</v>
       </c>
@@ -5326,7 +5889,7 @@
         <v>902.5</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1997</v>
       </c>
@@ -5352,7 +5915,7 @@
         <v>878.5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1998</v>
       </c>
@@ -5378,7 +5941,7 @@
         <v>827.3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -5404,7 +5967,7 @@
         <v>726.5</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2000</v>
       </c>
@@ -5430,7 +5993,7 @@
         <v>601.9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2001</v>
       </c>
@@ -5456,7 +6019,7 @@
         <v>768.5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2002</v>
       </c>
@@ -5482,7 +6045,7 @@
         <v>616.70000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B61">
         <f>B57/$H57</f>
         <v>0.53281275959461705</v>
@@ -5508,7 +6071,7 @@
         <v>3.8212327629174279E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B62">
         <f t="shared" ref="B62:G62" si="1">B58/$H58</f>
         <v>0.35836044242029924</v>
@@ -5534,7 +6097,7 @@
         <v>2.7325959661678597E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B63">
         <f t="shared" ref="B63:G63" si="2">B59/$H59</f>
         <v>0.39176260742662555</v>
@@ -5560,7 +6123,7 @@
         <v>3.2430679422733905E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65">
         <f>AVERAGE(B61:B63)</f>
         <v>0.42764526981384732</v>
@@ -5591,7 +6154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89270B2-663A-4EDF-A447-9DDCDB239B8B}">
   <dimension ref="A1:H35"/>
   <sheetViews>
@@ -5599,16 +6162,16 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5628,7 +6191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2007</v>
       </c>
@@ -5648,7 +6211,7 @@
         <v>40.94</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2008</v>
       </c>
@@ -5668,7 +6231,7 @@
         <v>44.65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2009</v>
       </c>
@@ -5688,7 +6251,7 @@
         <v>49.33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2010</v>
       </c>
@@ -5708,7 +6271,7 @@
         <v>42.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2011</v>
       </c>
@@ -5728,7 +6291,7 @@
         <v>49.96</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2012</v>
       </c>
@@ -5748,7 +6311,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2013</v>
       </c>
@@ -5768,7 +6331,7 @@
         <v>33.99</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2014</v>
       </c>
@@ -5788,7 +6351,7 @@
         <v>25.95</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2015</v>
       </c>
@@ -5808,7 +6371,7 @@
         <v>28.13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2016</v>
       </c>
@@ -5828,7 +6391,7 @@
         <v>29.25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2017</v>
       </c>
@@ -5848,7 +6411,7 @@
         <v>54.47</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2018</v>
       </c>
@@ -5871,7 +6434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -5900,7 +6463,7 @@
         <v>491.29999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -5925,12 +6488,12 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
@@ -5944,7 +6507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>B2/$F2</f>
         <v>0.55471421592574499</v>
@@ -5962,7 +6525,7 @@
         <v>3.2242305813385448E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" ref="B21:E21" si="3">B3/$F3</f>
         <v>0.56326987681970886</v>
@@ -5980,7 +6543,7 @@
         <v>2.8443449048152297E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22">
         <f t="shared" ref="B22:E22" si="4">B4/$F4</f>
         <v>0.61483884046219339</v>
@@ -5998,7 +6561,7 @@
         <v>2.4934117170079061E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23">
         <f t="shared" ref="B23:E23" si="5">B5/$F5</f>
         <v>0.55682613768961486</v>
@@ -6016,7 +6579,7 @@
         <v>2.7537922987164527E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24">
         <f t="shared" ref="B24:E24" si="6">B6/$F6</f>
         <v>0.60688550840672539</v>
@@ -6034,7 +6597,7 @@
         <v>2.2818254603682944E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25">
         <f t="shared" ref="B25:E25" si="7">B7/$F7</f>
         <v>0.62799145299145309</v>
@@ -6052,7 +6615,7 @@
         <v>1.217948717948718E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26">
         <f t="shared" ref="B26:E26" si="8">B8/$F8</f>
         <v>0.59958811415122093</v>
@@ -6070,7 +6633,7 @@
         <v>1.2062371285672255E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27">
         <f t="shared" ref="B27:E27" si="9">B9/$F9</f>
         <v>0.61040462427745668</v>
@@ -6088,7 +6651,7 @@
         <v>1.5414258188824664E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28">
         <f t="shared" ref="B28:E28" si="10">B10/$F10</f>
         <v>0.59936011375755416</v>
@@ -6106,7 +6669,7 @@
         <v>1.3864201919658729E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29">
         <f t="shared" ref="B29:E29" si="11">B11/$F11</f>
         <v>0.54188034188034184</v>
@@ -6124,7 +6687,7 @@
         <v>1.2649572649572649E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30">
         <f t="shared" ref="B30:E30" si="12">B12/$F12</f>
         <v>0.52138791995593903</v>
@@ -6142,7 +6705,7 @@
         <v>4.2225078024600701E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31">
         <f t="shared" ref="B31:E31" si="13">B13/$F13</f>
         <v>0.63828368163628291</v>
@@ -6160,7 +6723,7 @@
         <v>3.5571365051133841E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" ref="B32:E32" si="14">B14/$F14</f>
         <v>0.58579279462650091</v>
@@ -6178,7 +6741,7 @@
         <v>1.7647058823529408E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33">
         <f>B15/$F15</f>
         <v>0.58579279462650102</v>
@@ -6196,7 +6759,7 @@
         <v>1.7647058823529408E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -6222,7 +6785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C5C9BC-080A-4669-9D44-6DA444B28505}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -6230,27 +6793,27 @@
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F1">
         <f>SUM(A1:E1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F2">
         <f t="shared" ref="F2:F3" si="0">SUM(A2:E2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="e">
         <f>A1/$F1</f>
         <v>#DIV/0!</v>
@@ -6272,7 +6835,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="e">
         <f t="shared" ref="A6:E7" si="2">A2/$F2</f>
         <v>#DIV/0!</v>
@@ -6294,7 +6857,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
@@ -6316,7 +6879,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="e">
         <f>AVERAGE(A5:A7)</f>
         <v>#DIV/0!</v>
@@ -6343,7 +6906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC97E81-2628-4FD4-8A9D-220E7891A6E1}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -6351,27 +6914,27 @@
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F1">
         <f>SUM(A1:E1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F2">
         <f t="shared" ref="F2:F3" si="0">SUM(A2:E2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="e">
         <f>A1/$F1</f>
         <v>#DIV/0!</v>
@@ -6393,7 +6956,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="e">
         <f t="shared" ref="A6:E6" si="2">A2/$F2</f>
         <v>#DIV/0!</v>
@@ -6415,7 +6978,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="e">
         <f t="shared" ref="A7:D7" si="3">A3/$F3</f>
         <v>#DIV/0!</v>
@@ -6437,7 +7000,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="e">
         <f>AVERAGE(A5:A7)</f>
         <v>#DIV/0!</v>

</xml_diff>

<commit_message>
fraction of fishery calculation for canary rockfish
</commit_message>
<xml_diff>
--- a/data/Selectivity parameters/fraction_of_fishery.xlsx
+++ b/data/Selectivity parameters/fraction_of_fishery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vic\Documents\Projects\DensityRatio\data\Selectivity parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vic\Documents\Projects\MS-thesis\data\Selectivity parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596486B5-6927-4A06-8EA6-ED9D85229404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC715E-9E86-43DF-8040-0D82BD0D7EF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24825" yWindow="7260" windowWidth="13830" windowHeight="7170" xr2:uid="{61ABCC0D-E7EA-4BC2-A5B0-7613055FF009}"/>
+    <workbookView xWindow="28680" yWindow="-5700" windowWidth="19440" windowHeight="15000" activeTab="6" xr2:uid="{61ABCC0D-E7EA-4BC2-A5B0-7613055FF009}"/>
   </bookViews>
   <sheets>
     <sheet name="LING2017" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="BR 2003" sheetId="5" r:id="rId4"/>
     <sheet name="CAB2019" sheetId="3" r:id="rId5"/>
     <sheet name="lingcod" sheetId="2" r:id="rId6"/>
-    <sheet name="copper rockfish" sheetId="1" r:id="rId7"/>
+    <sheet name="CR.OR.2015" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Years</t>
   </si>
@@ -154,12 +154,54 @@
   <si>
     <t>Total catch</t>
   </si>
+  <si>
+    <t xml:space="preserve">Non-Trawl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreational </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WA </t>
+  </si>
+  <si>
+    <t>Non-Trawl</t>
+  </si>
+  <si>
+    <t>Rec</t>
+  </si>
+  <si>
+    <t>Prop</t>
+  </si>
+  <si>
+    <t>Avg. Prop</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At-sea hake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research </t>
+  </si>
+  <si>
+    <t>Hake</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +232,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -211,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -229,6 +283,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F2C116-E186-401B-9D63-CD4A71AC94B0}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -843,217 +915,217 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18">
-        <f>B2/$F2</f>
+        <f t="shared" ref="B18:E29" si="0">B2/$F2</f>
         <v>0.2225089766606822</v>
       </c>
       <c r="C18">
-        <f>C2/$F2</f>
+        <f t="shared" si="0"/>
         <v>0.16273002692998204</v>
       </c>
       <c r="D18">
-        <f>D2/$F2</f>
+        <f t="shared" si="0"/>
         <v>0.21967571813285458</v>
       </c>
       <c r="E18">
-        <f>E2/$F2</f>
+        <f t="shared" si="0"/>
         <v>0.39508527827648116</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19">
-        <f>B3/$F3</f>
+        <f t="shared" si="0"/>
         <v>0.31751874948490427</v>
       </c>
       <c r="C19">
-        <f>C3/$F3</f>
+        <f t="shared" si="0"/>
         <v>0.21601054916073734</v>
       </c>
       <c r="D19">
-        <f>D3/$F3</f>
+        <f t="shared" si="0"/>
         <v>0.17081948298123678</v>
       </c>
       <c r="E19">
-        <f>E3/$F3</f>
+        <f t="shared" si="0"/>
         <v>0.29562374660036811</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
-        <f>B4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.31826457160462707</v>
       </c>
       <c r="C20">
-        <f>C4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.19933899112119433</v>
       </c>
       <c r="D20">
-        <f>D4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.19104837128532617</v>
       </c>
       <c r="E20">
-        <f>E4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.29134806598885249</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21">
-        <f>B5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.31956849241364466</v>
       </c>
       <c r="C21">
-        <f>C5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.24959647046163777</v>
       </c>
       <c r="D21">
-        <f>D5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.19049284407618636</v>
       </c>
       <c r="E21">
-        <f>E5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.24034219304853113</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22">
-        <f>B6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.28501295929257509</v>
       </c>
       <c r="C22">
-        <f>C6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.24842201555115109</v>
       </c>
       <c r="D22">
-        <f>D6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.22640646440006099</v>
       </c>
       <c r="E22">
-        <f>E6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.24015856075621286</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23">
-        <f>B7/$F7</f>
+        <f t="shared" si="0"/>
         <v>0.25055582406959886</v>
       </c>
       <c r="C23">
-        <f>C7/$F7</f>
+        <f t="shared" si="0"/>
         <v>0.15215079748670854</v>
       </c>
       <c r="D23">
-        <f>D7/$F7</f>
+        <f t="shared" si="0"/>
         <v>0.29460286772998229</v>
       </c>
       <c r="E23">
-        <f>E7/$F7</f>
+        <f t="shared" si="0"/>
         <v>0.30269051071371028</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24">
-        <f>B8/$F8</f>
+        <f t="shared" si="0"/>
         <v>0.49392677273757035</v>
       </c>
       <c r="C24">
-        <f>C8/$F8</f>
+        <f t="shared" si="0"/>
         <v>0.10044786783542163</v>
       </c>
       <c r="D24">
-        <f>D8/$F8</f>
+        <f t="shared" si="0"/>
         <v>0.20525242667689036</v>
       </c>
       <c r="E24">
-        <f>E8/$F8</f>
+        <f t="shared" si="0"/>
         <v>0.2003903595141418</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25">
-        <f>B9/$F9</f>
+        <f t="shared" si="0"/>
         <v>0.52150402414486929</v>
       </c>
       <c r="C25">
-        <f>C9/$F9</f>
+        <f t="shared" si="0"/>
         <v>9.0641068634026392E-2</v>
       </c>
       <c r="D25">
-        <f>D9/$F9</f>
+        <f t="shared" si="0"/>
         <v>0.17091437513972726</v>
       </c>
       <c r="E25">
-        <f>E9/$F9</f>
+        <f t="shared" si="0"/>
         <v>0.21692655935613683</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26">
-        <f>B10/$F10</f>
+        <f t="shared" si="0"/>
         <v>0.45613346666497895</v>
       </c>
       <c r="C26">
-        <f>C10/$F10</f>
+        <f t="shared" si="0"/>
         <v>9.9163301730357853E-2</v>
       </c>
       <c r="D26">
-        <f>D10/$F10</f>
+        <f t="shared" si="0"/>
         <v>0.16116251693016542</v>
       </c>
       <c r="E26">
-        <f>E10/$F10</f>
+        <f t="shared" si="0"/>
         <v>0.28354071467449782</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27">
-        <f>B11/$F11</f>
+        <f t="shared" si="0"/>
         <v>0.35232665489707005</v>
       </c>
       <c r="C27">
-        <f>C11/$F11</f>
+        <f t="shared" si="0"/>
         <v>0.13313681346269093</v>
       </c>
       <c r="D27">
-        <f>D11/$F11</f>
+        <f t="shared" si="0"/>
         <v>0.22931277433148153</v>
       </c>
       <c r="E27">
-        <f>E11/$F11</f>
+        <f t="shared" si="0"/>
         <v>0.28520756061612224</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28">
-        <f>B12/$F12</f>
+        <f t="shared" si="0"/>
         <v>0.20577530948153186</v>
       </c>
       <c r="C28">
-        <f>C12/$F12</f>
+        <f t="shared" si="0"/>
         <v>0.16691223695643959</v>
       </c>
       <c r="D28">
-        <f>D12/$F12</f>
+        <f t="shared" si="0"/>
         <v>0.34247610412180285</v>
       </c>
       <c r="E28">
-        <f>E12/$F12</f>
+        <f t="shared" si="0"/>
         <v>0.28482375609203214</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29">
-        <f>B13/$F13</f>
+        <f t="shared" si="0"/>
         <v>0.30360526923965797</v>
       </c>
       <c r="C29">
-        <f>C13/$F13</f>
+        <f t="shared" si="0"/>
         <v>0.11360064709960713</v>
       </c>
       <c r="D29">
-        <f>D13/$F13</f>
+        <f t="shared" si="0"/>
         <v>0.40407903859486943</v>
       </c>
       <c r="E29">
-        <f>E13/$F13</f>
+        <f t="shared" si="0"/>
         <v>0.1787150450658655</v>
       </c>
     </row>
@@ -1066,15 +1138,15 @@
         <v>0.28723574453941997</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:E31" si="0">AVERAGE(C27:C29)</f>
+        <f t="shared" ref="C31:E31" si="1">AVERAGE(C27:C29)</f>
         <v>0.1378832325062459</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.32528930568271797</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24958212059133991</v>
       </c>
     </row>
@@ -6908,121 +6980,1105 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC97E81-2628-4FD4-8A9D-220E7891A6E1}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F1">
-        <f>SUM(A1:E1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F2">
-        <f t="shared" ref="F2:F3" si="0">SUM(A2:E2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="e">
-        <f>A1/$F1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B5" t="e">
-        <f t="shared" ref="B5:E5" si="1">B1/$F1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" t="e">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>2012</v>
+      </c>
+      <c r="B2" s="11">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="10">
+        <f>SUM(B2:F2)</f>
+        <v>12.8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2013</v>
+      </c>
+      <c r="B3" s="11">
+        <v>5.9</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5.2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G4" si="0">SUM(B3:F3)</f>
+        <v>15.100000000000001</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="12"/>
+      <c r="N3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="D4" s="11">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2006</v>
+      </c>
+      <c r="J4" s="8">
+        <v>7</v>
+      </c>
+      <c r="K4" s="8">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L4" s="12">
+        <v>12.8</v>
+      </c>
+      <c r="M4" s="12"/>
+      <c r="N4" s="8">
+        <v>3</v>
+      </c>
+      <c r="O4" s="8">
+        <v>2</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="8">
+        <v>6.8</v>
+      </c>
+      <c r="S4" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="T4" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I5" s="8">
+        <v>2007</v>
+      </c>
+      <c r="J5" s="8">
+        <v>12.1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="L5" s="12">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M5" s="12"/>
+      <c r="N5" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="O5" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="S5" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <f>B2/$G2</f>
+        <v>0.3828125</v>
+      </c>
+      <c r="C6">
+        <f>C2/$G2</f>
+        <v>0.2890625</v>
+      </c>
+      <c r="D6">
+        <f>D2/$G2</f>
+        <v>0.2890625</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:F6" si="1">E2/$G2</f>
+        <v>2.3437499999999997E-2</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="e">
-        <f t="shared" ref="A6:E6" si="2">A2/$F2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B6" t="e">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2008</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K6" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="L6" s="12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M6" s="12"/>
+      <c r="N6" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="O6" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="P6" s="12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="S6" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T6" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f>B3/$G3</f>
+        <v>0.39072847682119205</v>
+      </c>
+      <c r="C7">
+        <f>C3/$G3</f>
+        <v>0.3443708609271523</v>
+      </c>
+      <c r="D7">
+        <f>D3/$G3</f>
+        <v>0.22516556291390727</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:F7" si="2">E3/$G3</f>
+        <v>3.3112582781456949E-2</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="e">
-        <f t="shared" ref="A7:D7" si="3">A3/$F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B7" t="e">
+        <v>6.6225165562913907E-3</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2009</v>
+      </c>
+      <c r="J7" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L7" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="M7" s="12"/>
+      <c r="N7" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="O7" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="P7" s="12">
+        <v>3.4</v>
+      </c>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="8">
+        <v>19</v>
+      </c>
+      <c r="S7" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="T7" s="8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>B4/$G4</f>
+        <v>0.39893617021276595</v>
+      </c>
+      <c r="C8">
+        <f>C4/$G4</f>
+        <v>0.30319148936170215</v>
+      </c>
+      <c r="D8">
+        <f>D4/$G4</f>
+        <v>0.15957446808510636</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:F8" si="3">E4/$G4</f>
+        <v>3.1914893617021274E-2</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="e">
-        <f>E3/$F3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="e">
-        <f>AVERAGE(A5:A7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B9" t="e">
-        <f t="shared" ref="B9:D9" si="4">AVERAGE(B5:B7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" t="e">
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2010</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="L8" s="12">
+        <v>6.9</v>
+      </c>
+      <c r="M8" s="12"/>
+      <c r="N8" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="O8" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="P8" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="8">
+        <v>15.8</v>
+      </c>
+      <c r="S8" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I9" s="8">
+        <v>2011</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="K9" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="L9" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="8">
+        <v>9</v>
+      </c>
+      <c r="O9" s="8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="P9" s="12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="8">
+        <v>20.9</v>
+      </c>
+      <c r="S9" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="T9" s="8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B6:B8)</f>
+        <v>0.39082571567798602</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D10" si="4">AVERAGE(C6:C8)</f>
+        <v>0.31220828342961815</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" t="e">
-        <f>AVERAGE(E5:E7)</f>
-        <v>#DIV/0!</v>
+        <v>0.2246008436663379</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:F10" si="5">AVERAGE(E6:E8)</f>
+        <v>2.9488325466159409E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>4.2876831759898544E-2</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2012</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="K10" s="13">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L10" s="12">
+        <v>5.2</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="O10" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="P10" s="12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="S10" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="T10" s="8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I11" s="8">
+        <v>2013</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K11" s="13">
+        <v>5.9</v>
+      </c>
+      <c r="L11" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M11" s="12"/>
+      <c r="N11" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="O11" s="13">
+        <v>5.2</v>
+      </c>
+      <c r="P11" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S11" s="13">
+        <v>3.4</v>
+      </c>
+      <c r="T11" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I12" s="8">
+        <v>2014</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2</v>
+      </c>
+      <c r="K12" s="13">
+        <v>7.5</v>
+      </c>
+      <c r="L12" s="12">
+        <v>1.7</v>
+      </c>
+      <c r="M12" s="12"/>
+      <c r="N12" s="8">
+        <v>6.1</v>
+      </c>
+      <c r="O12" s="13">
+        <v>5.7</v>
+      </c>
+      <c r="P12" s="12">
+        <v>5.7</v>
+      </c>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S12" s="13">
+        <v>3</v>
+      </c>
+      <c r="T12" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="12"/>
+      <c r="N16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I17" s="9">
+        <v>2002</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="L17" s="12">
+        <v>3</v>
+      </c>
+      <c r="M17" s="12"/>
+      <c r="N17" s="9">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="9">
+        <v>0</v>
+      </c>
+      <c r="S17" s="9">
+        <v>0</v>
+      </c>
+      <c r="T17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I18" s="9">
+        <v>2003</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="M18" s="12"/>
+      <c r="N18" s="9">
+        <v>0</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="S18" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I19" s="9">
+        <v>2004</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="9">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="S19" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="T19" s="9">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I20" s="9">
+        <v>2005</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1</v>
+      </c>
+      <c r="M20" s="12"/>
+      <c r="N20" s="9">
+        <v>0</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="S20" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="T20" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I21" s="9">
+        <v>2006</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="M21" s="12"/>
+      <c r="N21" s="9">
+        <v>0</v>
+      </c>
+      <c r="O21" s="9">
+        <v>0</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="S21" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="T21" s="9">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I22" s="9">
+        <v>2007</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>2</v>
+      </c>
+      <c r="L22" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="M22" s="12"/>
+      <c r="N22" s="9">
+        <v>0</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="S22" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="T22" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I23" s="9">
+        <v>2008</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="L23" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="S23" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="T23" s="9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I24" s="9">
+        <v>2009</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="L24" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="N24" s="9">
+        <v>0</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0</v>
+      </c>
+      <c r="P24" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="S24" s="9">
+        <v>0</v>
+      </c>
+      <c r="T24" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I25" s="9">
+        <v>2010</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L25" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="9">
+        <v>0</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+      <c r="P25" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="9">
+        <v>0</v>
+      </c>
+      <c r="S25" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="T25" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I26" s="9">
+        <v>2011</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L26" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="9">
+        <v>0</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0</v>
+      </c>
+      <c r="P26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="9">
+        <v>0</v>
+      </c>
+      <c r="S26" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="T26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I27" s="9">
+        <v>2012</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="L27" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="M27" s="12"/>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="9">
+        <v>0</v>
+      </c>
+      <c r="S27" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="T27" s="9">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="28" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I28" s="9">
+        <v>2013</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L28" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="M28" s="12"/>
+      <c r="N28" s="9">
+        <v>0</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0</v>
+      </c>
+      <c r="P28" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="S28" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="T28" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I29" s="9">
+        <v>2014</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="L29" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="M29" s="12"/>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+      <c r="P29" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="S29" s="13">
+        <v>2</v>
+      </c>
+      <c r="T29" s="9">
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="54">
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="P10:Q10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>